<commit_message>
Push few changes in Non-Proforma script and push till now complete script for Proforma
</commit_message>
<xml_diff>
--- a/src/test/java/com/test/ISAlbi/testData/ConfigurationSettings.xlsx
+++ b/src/test/java/com/test/ISAlbi/testData/ConfigurationSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Albi\ISAlbi_Automation\src\test\java\com\test\ISAlbi\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E10E26-E74D-451C-A665-C67C07FBDF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E5F8B4-F189-4DEB-B875-80948EDB39A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -68,26 +68,26 @@
     <t>SENT_FROM</t>
   </si>
   <si>
-    <t>sibesh@zanui.com</t>
-  </si>
-  <si>
     <t>Automation Test Report</t>
   </si>
   <si>
     <t>localhost</t>
   </si>
   <si>
-    <t>noreply@zanui.com</t>
-  </si>
-  <si>
     <t>Firefox</t>
+  </si>
+  <si>
+    <t>lalita.kashyaponestop@gmail.com</t>
+  </si>
+  <si>
+    <t>noreply@isalbi.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +102,11 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF5F6368"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,10 +130,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -407,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -443,7 +449,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -484,13 +490,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.77734375" customWidth="1"/>
     <col min="3" max="3" width="12.77734375" customWidth="1"/>
     <col min="4" max="4" width="17.44140625" customWidth="1"/>
@@ -511,23 +517,24 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{054F3F6E-7C08-43E0-B4B0-569E8C5B2D83}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>